<commit_message>
tracker update for 13 feb 2022
</commit_message>
<xml_diff>
--- a/Output Data/snapshot_graphs.xlsx
+++ b/Output Data/snapshot_graphs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vibhav/Documents/Projects/nimf-tracker-git/nimf-tracker/Manual/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vibhav/Documents/Projects/nimf-tracker-git/nimf-tracker/Output Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54941F71-D8EC-8A4D-AF8D-A25E357926AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{649B51CF-D993-6647-8BA7-38AE2EE809C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34140" yWindow="500" windowWidth="17060" windowHeight="9960" xr2:uid="{729EB3FA-4BB2-534E-B78E-282A2D9A819C}"/>
   </bookViews>
@@ -678,7 +678,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>26-Jan-22</c:v>
+                  <c:v>09-Feb-22</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -725,19 +725,19 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-0.02</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.05</c:v>
+                  <c:v>0.14000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.04</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.41</c:v>
+                  <c:v>0.52</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.17</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1834,8 +1834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{759904DE-AEA7-D24F-B06C-CD1A3C0BFC8A}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1991,22 +1991,22 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
-        <v>44587</v>
+        <v>44601</v>
       </c>
       <c r="B8" s="5">
-        <v>-0.02</v>
+        <v>0.04</v>
       </c>
       <c r="C8" s="5">
-        <v>-0.05</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="D8" s="5">
-        <v>-0.04</v>
+        <v>0.05</v>
       </c>
       <c r="E8" s="5">
-        <v>0.41</v>
+        <v>0.52</v>
       </c>
       <c r="F8" s="5">
-        <v>0.17</v>
+        <v>0.08</v>
       </c>
       <c r="G8" s="3"/>
     </row>

</xml_diff>